<commit_message>
Gains are all Found
I found all the gains for the selected operating points. They are now in a spreadsheet in the nonlinear double track folder
</commit_message>
<xml_diff>
--- a/MATLAB/nonlinear_double_track/pi_controller_gains.xlsx
+++ b/MATLAB/nonlinear_double_track/pi_controller_gains.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\School\_University of Akron\12th Semester - Spring 2025 (PC)\SDP\Vehicle-Dynamics\MATLAB\nonlinear_double_track\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA440DA-EAB5-4246-9256-3EDA9CA65FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED736C61-3514-4D51-B972-C2C114E546BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26505" yWindow="8700" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="6285" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -360,7 +360,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,6 +395,12 @@
       <c r="A2">
         <v>10</v>
       </c>
+      <c r="B2">
+        <v>25320</v>
+      </c>
+      <c r="C2">
+        <v>11396</v>
+      </c>
       <c r="D2">
         <v>8344.4</v>
       </c>
@@ -430,6 +436,18 @@
       <c r="A3">
         <v>20</v>
       </c>
+      <c r="B3">
+        <v>25320</v>
+      </c>
+      <c r="C3">
+        <v>11396</v>
+      </c>
+      <c r="D3">
+        <v>8300</v>
+      </c>
+      <c r="E3">
+        <v>12000</v>
+      </c>
       <c r="F3">
         <v>2483.6999999999998</v>
       </c>
@@ -459,6 +477,18 @@
       <c r="A4">
         <v>40</v>
       </c>
+      <c r="B4">
+        <v>25320</v>
+      </c>
+      <c r="C4">
+        <v>11396</v>
+      </c>
+      <c r="D4">
+        <v>8300</v>
+      </c>
+      <c r="E4">
+        <v>12000</v>
+      </c>
       <c r="F4">
         <v>2483.6999999999998</v>
       </c>
@@ -488,6 +518,18 @@
       <c r="A5">
         <v>60</v>
       </c>
+      <c r="B5">
+        <v>25320</v>
+      </c>
+      <c r="C5">
+        <v>11396</v>
+      </c>
+      <c r="D5">
+        <v>8300</v>
+      </c>
+      <c r="E5">
+        <v>12000</v>
+      </c>
       <c r="F5">
         <v>6836.2</v>
       </c>
@@ -516,6 +558,18 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>90</v>
+      </c>
+      <c r="B6">
+        <v>25320</v>
+      </c>
+      <c r="C6">
+        <v>11396</v>
+      </c>
+      <c r="D6">
+        <v>8300</v>
+      </c>
+      <c r="E6">
+        <v>12000</v>
       </c>
       <c r="F6">
         <v>6836.2</v>

</xml_diff>